<commit_message>
Update tokens file and get tokens from the token file
</commit_message>
<xml_diff>
--- a/src/assets/tokens.xlsx
+++ b/src/assets/tokens.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">userEmail</t>
   </si>
@@ -34,16 +34,18 @@
     <t xml:space="preserve">user_123</t>
   </si>
   <si>
-    <t xml:space="preserve">access_token_123</t>
+    <t xml:space="preserve">EAB3k2pU1ZBxwBO6ixHJeIO6kJu3wGOtPkyrUxA8zRL4ZAZAPrS6oLq1Nn0eXyDRKpc9aNO7cr9KsG7ZCAs23aTj7tlnwaZC3Mu5gOwZBRMQ2vRZCQK48vjx3L35Pm7biuICrf1s39CZAmExTlZBdOjJE3fxbtcMHwKIZBbDehr3hqdaeMvLp46jklc3UyB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EAAYEnKKz8boBO5oswUfODAELXCONlHCM3UDCBTcvWZBSUZAelyM17CUVW04DPHM7ZAya1NEgSipigLu32zHKXYVBuUVgGGay7SBzniPuvSYxzRFBV6VtmVzecB73CulCqK2ptnMGm7zJRifdRoQCbc3dg8c17AzoLgOwX8ZAYJWAsf7SdvB2lbndDUJZCnzyZAYkrjVZA6R</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -116,8 +118,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -137,17 +139,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.51171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="59.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="60.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -161,15 +163,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="79.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>45539.4305678588</v>
+        <v>1730486029253</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>1730491898045</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Send like, messages limit increase, attachments
</commit_message>
<xml_diff>
--- a/src/assets/tokens.xlsx
+++ b/src/assets/tokens.xlsx
@@ -34,10 +34,10 @@
     <t xml:space="preserve">user_123</t>
   </si>
   <si>
-    <t xml:space="preserve">EAB3k2pU1ZBxwBO6ixHJeIO6kJu3wGOtPkyrUxA8zRL4ZAZAPrS6oLq1Nn0eXyDRKpc9aNO7cr9KsG7ZCAs23aTj7tlnwaZC3Mu5gOwZBRMQ2vRZCQK48vjx3L35Pm7biuICrf1s39CZAmExTlZBdOjJE3fxbtcMHwKIZBbDehr3hqdaeMvLp46jklc3UyB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EAAYEnKKz8boBO5oswUfODAELXCONlHCM3UDCBTcvWZBSUZAelyM17CUVW04DPHM7ZAya1NEgSipigLu32zHKXYVBuUVgGGay7SBzniPuvSYxzRFBV6VtmVzecB73CulCqK2ptnMGm7zJRifdRoQCbc3dg8c17AzoLgOwX8ZAYJWAsf7SdvB2lbndDUJZCnzyZAYkrjVZA6R</t>
+    <t xml:space="preserve">EAAYEnKKz8boBO5QAo8wfND3MaxQPcxC3E6ZAeVtPjag56fGuQj22Uu2qnAqgPzsOCuehwC5ZCr25DDstIoUiuArIpAPaRZBdMddZB4ciwUkuaZCNNWdKFM7jX02mQbIeSduZCDyNGl9or57ZCk3MdOq0sQ4jPNYXhiHdZCF7VdBeme7qKmTqjrZCJ6oHWVGIgtwTqq3h9lol8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EAAYEnKKz8boBO6gZBHNfPuB6KjaALlsV1fNVrZCIKCRU5hov97XsMqiTsRfVOd1pD3oZAIaehO32g7HDCivbY8WXIHcEWVxwxPNHZAobXfF4xsZCUvSEzzLioeQTWS0g71iJZAZCBbMkj4caSmRd1jhM7ygPGzdhHr2Jp4wQPfRXBLUp6PIdLUtvt5E</t>
   </si>
 </sst>
 </file>
@@ -113,9 +113,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -142,21 +150,21 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.51171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="59.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="59.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="60.51"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
@@ -167,18 +175,18 @@
       <c r="A2" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="C2" s="3" t="n">
         <v>1730486029253</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="1" t="s">
+    <row r="3" customFormat="false" ht="137.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="3" t="n">
         <v>1730491898045</v>
       </c>
     </row>

</xml_diff>